<commit_message>
Updated penalty stats for GW21
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EB3541-F115-4AFD-A7C2-A6DC96C8E79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F2625A-55F0-4E99-B711-0C272AA97BA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,13 +94,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,8 +395,8 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,9 +656,12 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>21</v>
       </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
Updated league table for GW21.
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F2625A-55F0-4E99-B711-0C272AA97BA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E443DEC-2D55-44CA-AA83-7FBEABCBDCBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,6 +654,15 @@
       <c r="A18" s="1">
         <v>20</v>
       </c>
+      <c r="B18">
+        <v>104</v>
+      </c>
+      <c r="C18">
+        <v>127</v>
+      </c>
+      <c r="D18">
+        <v>132</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -774,15 +783,15 @@
       </c>
       <c r="B41">
         <f>SUM(B2:B40)</f>
-        <v>1242</v>
+        <v>1346</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="0">SUM(C2:C40)</f>
-        <v>1384</v>
+        <v>1511</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1162</v>
+        <v>1294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated league table for GW22.
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB039A92-2E46-479B-9BD5-015032508C98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33C383B-F5EB-4540-8321-960FD5021689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,9 +394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,9 +668,15 @@
       <c r="A19" s="2">
         <v>21</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="3">
+        <v>105</v>
+      </c>
+      <c r="C19" s="3">
+        <v>115</v>
+      </c>
+      <c r="D19" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -783,15 +789,15 @@
       </c>
       <c r="B41">
         <f>SUM(B2:B40)</f>
-        <v>1346</v>
+        <v>1451</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="0">SUM(C2:C40)</f>
-        <v>1511</v>
+        <v>1626</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1294</v>
+        <v>1384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated league table for GW23.
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33C383B-F5EB-4540-8321-960FD5021689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDFA799-5B34-42E9-82F6-85F705BF33E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,11 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,16 +395,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -682,6 +683,15 @@
       <c r="A20" s="1">
         <v>22</v>
       </c>
+      <c r="B20" s="4">
+        <v>110</v>
+      </c>
+      <c r="C20" s="4">
+        <v>78</v>
+      </c>
+      <c r="D20" s="4">
+        <v>99</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -789,15 +799,15 @@
       </c>
       <c r="B41">
         <f>SUM(B2:B40)</f>
-        <v>1451</v>
+        <v>1561</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="0">SUM(C2:C40)</f>
-        <v>1626</v>
+        <v>1704</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1384</v>
+        <v>1483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated league table for GW24.
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDFA799-5B34-42E9-82F6-85F705BF33E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85FADB2-20E5-4032-ABEA-33C207486380}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,6 +697,15 @@
       <c r="A21" s="1">
         <v>23</v>
       </c>
+      <c r="B21" s="4">
+        <v>99</v>
+      </c>
+      <c r="C21" s="4">
+        <v>106</v>
+      </c>
+      <c r="D21" s="4">
+        <v>72</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -799,15 +808,15 @@
       </c>
       <c r="B41">
         <f>SUM(B2:B40)</f>
-        <v>1561</v>
+        <v>1660</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="0">SUM(C2:C40)</f>
-        <v>1704</v>
+        <v>1810</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1483</v>
+        <v>1555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated league table for GW25.
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85FADB2-20E5-4032-ABEA-33C207486380}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02A8DC-7B30-4B6A-8774-61A13F627249}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,6 +711,15 @@
       <c r="A22" s="1">
         <v>24</v>
       </c>
+      <c r="B22" s="4">
+        <v>92</v>
+      </c>
+      <c r="C22" s="4">
+        <v>93</v>
+      </c>
+      <c r="D22" s="4">
+        <v>98</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -808,15 +817,15 @@
       </c>
       <c r="B41">
         <f>SUM(B2:B40)</f>
-        <v>1660</v>
+        <v>1752</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="0">SUM(C2:C40)</f>
-        <v>1810</v>
+        <v>1903</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1555</v>
+        <v>1653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated league table for GW26.
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02A8DC-7B30-4B6A-8774-61A13F627249}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB1DD6-3465-4337-8933-DF9218393597}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +725,15 @@
       <c r="A23" s="1">
         <v>25</v>
       </c>
+      <c r="B23" s="4">
+        <v>87</v>
+      </c>
+      <c r="C23" s="4">
+        <v>99</v>
+      </c>
+      <c r="D23" s="4">
+        <v>103</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -817,15 +826,15 @@
       </c>
       <c r="B41">
         <f>SUM(B2:B40)</f>
-        <v>1752</v>
+        <v>1839</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="0">SUM(C2:C40)</f>
-        <v>1903</v>
+        <v>2002</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1653</v>
+        <v>1756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated league table for GW27.
</commit_message>
<xml_diff>
--- a/league_table.xlsx
+++ b/league_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\PycharmProjects\pososyal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB1DD6-3465-4337-8933-DF9218393597}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE1582B-E570-4D53-B7B3-9165991D46DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,6 +739,15 @@
       <c r="A24" s="1">
         <v>26</v>
       </c>
+      <c r="B24" s="4">
+        <v>83</v>
+      </c>
+      <c r="C24" s="4">
+        <v>72</v>
+      </c>
+      <c r="D24" s="4">
+        <v>82</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -826,15 +835,15 @@
       </c>
       <c r="B41">
         <f>SUM(B2:B40)</f>
-        <v>1839</v>
+        <v>1922</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="0">SUM(C2:C40)</f>
-        <v>2002</v>
+        <v>2074</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1756</v>
+        <v>1838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>